<commit_message>
Add simulation functionality and logging to the game
- Implemented the main simulation logic in `simulador.py`, allowing players to simulate multiple rounds of the game.
- Introduced a `Logger` class to track game events and player actions.
- Updated `main.py` to allow users to choose between combined and random decks.
- Enhanced `datos_rulkanis.py` with equipment distribution data.
- Created new `mazo.py` for deck construction functions.
- Added `event.py` and `logger.py` for event handling and logging functionality.
</commit_message>
<xml_diff>
--- a/resultados_simulacion.xlsx
+++ b/resultados_simulacion.xlsx
@@ -468,19 +468,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ARMA: Karsuk Jairuk, BOTAS: Exilte Naor, CASCO: Nishuk Ashai, PECHERA: Exilte Naor, GUANTES: Karsuk Jairuk</t>
+          <t>ARMA: Rougur Ivaiesk, BOTAS: Karsuk Jairuk, CASCO: Exilte Naor, PECHERA: Nishuk Ashai, GUANTES: Karsuk Jairuk</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ataque critico + paralizar certero, ATAQUE NORMAL + SANGRADO AZAR, Sangrado certero + buffo defensa, ATAQUE CRITICO, ATAQUE NORMAL + FUEGO AZAR, ATAQUE NORMAL, FUEGO CERTERO, BUFFO DEFENSA NORMAL, ATAQUE LIGERO, PARALIZAR AZAR, BUFFO DEFENSA, Ataque ligero + congelar azar, Fuego azar + paralizar azar , PARALIZAR AZAR, BUFFO SUERTE, Ataque ligero + robo de carta, ATAQUE LIGERO, ATAQUE NORMAL + SANGRADO CERTERO, Ataque ligero + limpieza azar, BUFFO LIMPIEZA AZAR, ATAQUE NORMAL, ESQUIVAR AZAR, BUFFO VIDA PEQUEÑO, ATAQUE NORMAL, ATAQUE LIGERO, FUEGO AZAR, PARALIZAR AZAR, ATAQUE NORMAL, ESQUIVAR AZAR + ATAQUE LIGERO, SANGRADO CERTERO, BUFFO DEFENSA FUERTE, BUFFO VIDA MEDIANO, CONGELAR CERTERO, ATAQUE NORMAL + SANGRADO CERTERO, ATAQUE NORMAL PARALIZAR AZAR</t>
+          <t>Ataque critico + fuego certero, ATAQUE NORMAL + CONGELAR AZAR, Fuego certero +. Paralizar certero, ATAQUE CRITICO, BUFFO SUERTE, BUFFO LIMPIEZA AZAR, ATAQUE NORMAL, BUFFO DEFENSA NORMAL, Ataque ligero + fuego azar, Ataque ligero + paralizar azar, ATAQUE LIGERO, FUEGO AZAR, PARALIZAR AZAR, BUFFO DEFENSA, ESQUIVAR AZAR, BUFFO DEFENSA FUERTE, BUFFO DEFENSA NORMAL, ESQUIVAR AZAR, BUFFO SUERTE, ATAQUE LIGERO, Ataque critico + fuego certero, BUFFO VIDA MEDIANO, BUFFO LIMPIEZA AZAR, CONGELAR AZAR, ATAQUE LIGERO, PARALIZAR AZAR, BUFFO VIDA PEQUEÑO, ATAQUE NORMAL, ATAQUE LIGERO, FUEGO AZAR, PARALIZAR AZAR, ESQUIVAR AZAR + ATAQUE LIGERO, ATAQUE NORMAL, BUFFO DEFENSA FUERTE, ATAQUE CRITICO, BUFFO VIDA MEDIANO, ATAQUE NORMAL + SANGRADO AZAR, ATAQUE NORMAL + SANGRADO CERTERO, BUFFO VIDA GRANDE</t>
         </is>
       </c>
     </row>
@@ -491,19 +491,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ARMA: Exilte Naor, BOTAS: Karsuk Jairuk, CASCO: Exilte Naor, PECHERA: Nishuk Ashai, GUANTES: Exilte Naor</t>
+          <t>ARMA: Exilte Naor, BOTAS: Nishuk Ashai, CASCO: Karsuk Jairuk, PECHERA: Exilte Naor, GUANTES: Nishuk Ashai</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ataque critico + fuego certero, CONGELAR CERTERO, Ataque critico + robar carta, SANGRADO CERTERO, BUFFO LIMPIEZA AZAR, Ataque ligero + sangrado azar, ATAQUE NORMAL, SANGRADO AZAR, Ataque ligero + paralizar azar, ATAQUE LIGERO, BUFFO DEFENSA, BUFFO DEFENSA FUERTE, BUFFO DEFENSA NORMAL, ESQUIVAR AZAR, BUFFO SUERTE, ATAQUE LIGERO, Ataque critico + fuego certero, BUFFO VIDA MEDIANO, BUFFO LIMPIEZA AZAR, CONGELAR AZAR, ATAQUE CRITICO, BUFFO DEFENSA NORMAL, BUFFO DEFENSA, ATAQUE LIGERO, FUEGO AZAR, SANGRADO AZAR, ATAQUE NORMAL, ATAQUE CRITICO, SANGRADO CERTERO, ATAQUE NORMAL + SANGRADO AZAR, BUFFO VIDA MEDIANO, BUFFO VIDA GRANDE, ATAQUE NORMAL + SANGRADO CERTERO</t>
+          <t>Ataque critico + fuego certero, CONGELAR CERTERO, Ataque critico + robar carta, SANGRADO CERTERO, BUFFO LIMPIEZA AZAR, Ataque ligero + sangrado azar, ATAQUE NORMAL, SANGRADO AZAR, Ataque ligero + paralizar azar, ATAQUE LIGERO, BUFFO DEFENSA, BUFFO DEFENSA FUERTE, Fuego azar +buffo defensa, ESQUIVAR AZAR, BUFFO SUERTE, SANGRADO AZAR, ATAQUE LIGERO, ATAQUE NORMAL + SANGRADO CERTERO, Ataque ligero + limpieza azar, BUFFO LIMPIEZA AZAR, ATAQUE NORMAL, BUFFO DEFENSA, ESQUIVAR AZAR, BUFFO DEFENSA FUERTE, BUFFO DEFENSA NORMAL, BUFFO DEFENSA, ATAQUE LIGERO, FUEGO AZAR, SANGRADO AZAR, ESQUIVAR AZAR + ATAQUE LIGERO, SANGRADO CERTERO, BUFFO DEFENSA FUERTE, CONGELAR CERTERO, BUFFO VIDA MEDIANO, ATAQUE NORMAL PARALIZAR AZAR, BUFFO VIDA GRANDE</t>
         </is>
       </c>
     </row>
@@ -518,7 +518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,7 +605,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -661,25 +661,25 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>BUFFO VIDA GRANDE (Éxito) | Bufo Vida Grande: +3 vida (vida ahora 18)</t>
+          <t>ATAQUE NORMAL PARALIZAR AZAR (Éxito, dado=10) | Ataque Normal: 0 absorbido, 2 a vida (vida ahora 13) &amp; Paralizar Azar: fallido (dado=4)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
+        <v>13</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
         <v>15</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>18</v>
-      </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BUFFO VIDA GRANDE</t>
+          <t>ATAQUE NORMAL PARALIZAR AZAR</t>
         </is>
       </c>
       <c r="L3" t="n">
@@ -687,13 +687,11 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>AZAR</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>10</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -703,7 +701,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -716,25 +714,25 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>BUFFO LIMPIEZA AZAR (Éxito, dado=8) | Limpieza: estados negativos eliminados</t>
+          <t>SANGRADO CERTERO (Éxito) | Sangrado Certero: aplicado (1×3 turnos)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
+        <v>12</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>15</v>
       </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>18</v>
-      </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BUFFO LIMPIEZA AZAR</t>
+          <t>SANGRADO CERTERO</t>
         </is>
       </c>
       <c r="L4" t="n">
@@ -742,11 +740,13 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>AZAR</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>8</v>
+          <t>CERTERO</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -769,37 +769,39 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Ataque ligero + paralizar azar (Éxito, dado=9) | Ataque Ligero: 0 absorbido, 1 a vida (vida ahora 14) &amp; Paralizar Azar: aplicado (dado=9, 2 turnos)</t>
+          <t>BUFFO DEFENSA (Éxito) | Bufo Defensa: +1 defensa</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Ataque ligero + paralizar azar</t>
+          <t>BUFFO DEFENSA</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>AZAR</t>
-        </is>
-      </c>
-      <c r="N5" t="n">
-        <v>9</v>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -809,7 +811,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -826,23 +828,23 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Paralizado: dado 9 (≥6), puede jugar</t>
+          <t>S; a; n; g; r; a; d; o; :;  ; -; 1;  ; v; i; d; a</t>
         </is>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -852,62 +854,56 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="n">
         <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Jugador 1</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Reaccion</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>BUFFO VIDA PEQUEÑO (Éxito) | Bufo Vida Pequeño: +1 vida (vida ahora 15)</t>
+          <t>Ataque ligero + paralizar azar (Éxito, dado=10) | REACCIÓN: Jugador 2 juega ESQUIVAR AZAR → Esquivar Azar: fallido (dado=3)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
+        <v>11</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
         <v>15</v>
       </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>18</v>
-      </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BUFFO VIDA PEQUEÑO</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>3</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+          <t>ESQUIVAR AZAR</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Éxito</t>
+          <t>Fallido</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -920,33 +916,33 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>FUEGO CERTERO (Éxito) | Fuego Certero: aplicado (1×3 turnos)</t>
+          <t>ATAQUE LIGERO (Éxito) | Ataque Ligero: 1 absorbido por defensa (defensa ahora 0)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
+        <v>11</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
         <v>15</v>
       </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>17</v>
-      </c>
       <c r="J8" t="n">
         <v>0</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>FUEGO CERTERO</t>
+          <t>ATAQUE LIGERO</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>CERTERO</t>
+          <t>NORMAL</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -962,7 +958,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="n">
         <v>2</v>
@@ -975,12 +971,12 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ATAQUE NORMAL (Éxito) | Ataque Normal: 0 absorbido, 2 a vida (vida ahora 15)</t>
+          <t>FUEGO AZAR (Éxito, dado=10) | Fuego Azar: fallido (dado=2)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -993,21 +989,19 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>ATAQUE NORMAL</t>
+          <t>FUEGO AZAR</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>AZAR</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>10</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1017,7 +1011,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="n">
         <v>3</v>
@@ -1034,20 +1028,20 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Fuego: -1 vida</t>
+          <t>—</t>
         </is>
       </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
       <c r="G10" t="n">
+        <v>11</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
         <v>15</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>14</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -1060,7 +1054,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="n">
         <v>3</v>
@@ -1073,39 +1067,37 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ATAQUE CRITICO (Éxito) | Ataque Crítico: 0 absorbido, 3 a vida (vida ahora 12)</t>
+          <t>FUEGO AZAR (Éxito, dado=9) | Fuego Azar: fallido (dado=2)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>ATAQUE CRITICO</t>
+          <t>FUEGO AZAR</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>AZAR</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>9</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1115,60 +1107,50 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Jugador 2</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>FUEGO AZAR (Éxito, dado=6) | Fuego Azar: fallido (dado=4)</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
+          <t>S; a; n; g; r; a; d; o; :;  ; -; 1;  ; v; i; d; a</t>
+        </is>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
       <c r="G12" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>FUEGO AZAR</t>
-        </is>
-      </c>
-      <c r="L12" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>AZAR</t>
-        </is>
-      </c>
-      <c r="N12" t="n">
-        <v>6</v>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>Éxito</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="n">
         <v>4</v>
@@ -1178,21 +1160,15 @@
           <t>Jugador 1</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>InicioTurno</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Paralizado: dado 10 (≥6), puede jugar</t>
-        </is>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
+          <t>ATAQUE LIGERO (Éxito) | Ataque Ligero: 0 absorbido, 1 a vida (vida ahora 14)</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1203,113 +1179,121 @@
       <c r="J13" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>ATAQUE LIGERO</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Jugador 1</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Ataque critico + paralizar certero (Éxito) | Ataque Crítico: 0 absorbido, 3 a vida (vida ahora 11) &amp; Paralizar Certero: aplicado (2 turnos)</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
       <c r="G14" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Ataque critico + paralizar certero</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>5</v>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>CERTERO</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>Éxito</t>
-        </is>
-      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Jugador 1</t>
+          <t>Jugador 2</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>FUEGO AZAR (Éxito, dado=9) | Fuego Azar: fallido (dado=2)</t>
+          <t>BUFFO VIDA GRANDE (Éxito) | Bufo Vida Grande: +3 vida (vida ahora 17)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>FUEGO AZAR</t>
+          <t>BUFFO VIDA GRANDE</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>AZAR</t>
-        </is>
-      </c>
-      <c r="N15" t="n">
-        <v>9</v>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1319,14 +1303,14 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Jugador 2</t>
+          <t>Jugador 1</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1336,20 +1320,20 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Fuego: -1 vida; Paralizado: dado 10 (≥6), puede jugar</t>
+          <t>S; a; n; g; r; a; d; o; :;  ; -; 1;  ; v; i; d; a</t>
         </is>
       </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1362,31 +1346,31 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Jugador 2</t>
+          <t>Jugador 1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>ATAQUE LIGERO (Éxito) | Ataque Ligero: 0 absorbido, 1 a vida (vida ahora 11)</t>
+          <t>ATAQUE LIGERO (Éxito) | Ataque Ligero: 0 absorbido, 1 a vida (vida ahora 16)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
@@ -1417,161 +1401,151 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>Jugador 2</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>BUFFO DEFENSA (Éxito) | Bufo Defensa: +1 defensa</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
       <c r="G18" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J18" t="n">
-        <v>1</v>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>BUFFO DEFENSA</t>
-        </is>
-      </c>
-      <c r="L18" t="n">
-        <v>1</v>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>Éxito</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Jugador 1</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>InicioTurno</t>
-        </is>
-      </c>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
+          <t>CONGELAR CERTERO (Éxito) | Congelar Certero: aplicado (salta turno)</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
-      </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>CONGELAR CERTERO</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>4</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>CERTERO</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>Jugador 1</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>PARALIZAR AZAR (Éxito, dado=10) | Paralizar Azar: aplicado (dado=8, 2 turnos)</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
+          <t>C; o; n; g; e; l; a; d; o; :;  ; p; i; e; r; d; e;  ; t; u; r; n; o</t>
+        </is>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
       <c r="G20" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>PARALIZAR AZAR</t>
-        </is>
-      </c>
-      <c r="L20" t="n">
-        <v>1</v>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>AZAR</t>
-        </is>
-      </c>
-      <c r="N20" t="n">
-        <v>10</v>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>Éxito</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1585,20 +1559,20 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Fuego: -1 defensa; Paralizado: dado 10 (≥6), puede jugar</t>
+          <t>—</t>
         </is>
       </c>
       <c r="F21" t="b">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -1611,82 +1585,66 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Jugador 2</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>SANGRADO AZAR (Éxito, dado=8) | Sangrado Azar: aplicado (dado=10, 1×3 turnos)</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
       <c r="G22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>SANGRADO AZAR</t>
-        </is>
-      </c>
-      <c r="L22" t="n">
-        <v>2</v>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>AZAR</t>
-        </is>
-      </c>
-      <c r="N22" t="n">
-        <v>8</v>
-      </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>Éxito</t>
-        </is>
-      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>Jugador 1</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>InicioTurno</t>
-        </is>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Sangrado: -1 vida</t>
-        </is>
-      </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
+          <t>ATAQUE NORMAL (Éxito) | Ataque Normal: 0 absorbido, 2 a vida (vida ahora 14)</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
         <v>9</v>
       </c>
@@ -1694,36 +1652,60 @@
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
       </c>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>ATAQUE NORMAL</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>2</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Jugador 1</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ATAQUE LIGERO (Éxito) | Ataque Ligero: 0 absorbido, 1 a vida (vida ahora 9)</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr"/>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
       <c r="G24" t="n">
         <v>9</v>
       </c>
@@ -1731,60 +1713,36 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>ATAQUE LIGERO</t>
-        </is>
-      </c>
-      <c r="L24" t="n">
-        <v>1</v>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>Éxito</t>
-        </is>
-      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>Jugador 2</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>InicioTurno</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Paralizado: dado 2 (&lt;6), pierde turno</t>
-        </is>
-      </c>
-      <c r="F25" t="b">
-        <v>1</v>
-      </c>
+          <t>BUFFO LIMPIEZA AZAR (Éxito, dado=6) | Limpieza: estados negativos eliminados</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
         <v>9</v>
       </c>
@@ -1792,23 +1750,39 @@
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>BUFFO LIMPIEZA AZAR</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>3</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>AZAR</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>6</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1822,20 +1796,20 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Sangrado: -1 vida</t>
+          <t>—</t>
         </is>
       </c>
       <c r="F26" t="b">
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J26" t="n">
         <v>0</v>
@@ -1848,10 +1822,10 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1861,37 +1835,39 @@
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>ATAQUE NORMAL + FUEGO AZAR (Éxito, dado=6) | Ataque Normal: 0 absorbido, 2 a vida (vida ahora 7) &amp; Fuego Azar: aplicado (dado=8, 1×3 turnos)</t>
+          <t>Ataque critico + fuego certero (Éxito) | Ataque Crítico: 0 absorbido, 3 a vida (vida ahora 11) &amp; Fuego Certero: aplicado (1×3 turnos)</t>
         </is>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J27" t="n">
         <v>0</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>ATAQUE NORMAL + FUEGO AZAR</t>
+          <t>Ataque critico + fuego certero</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>AZAR</t>
-        </is>
-      </c>
-      <c r="N27" t="n">
-        <v>6</v>
+          <t>CERTERO</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -1901,10 +1877,10 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1918,20 +1894,20 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Fuego: -1 vida</t>
+          <t>F; u; e; g; o; :;  ; -; 1;  ; v; i; d; a</t>
         </is>
       </c>
       <c r="F28" t="b">
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J28" t="n">
         <v>0</v>
@@ -1944,10 +1920,10 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1957,33 +1933,33 @@
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Ataque critico + fuego certero (Éxito) | Ataque Crítico: 0 absorbido, 3 a vida (vida ahora 5) &amp; Fuego Certero: aplicado (1×3 turnos)</t>
+          <t>ATAQUE NORMAL (Éxito) | Ataque Normal: 0 absorbido, 2 a vida (vida ahora 7)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Ataque critico + fuego certero</t>
+          <t>ATAQUE NORMAL</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>CERTERO</t>
+          <t>NORMAL</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
@@ -1999,10 +1975,10 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -2016,20 +1992,20 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Sangrado: -1 vida; Fuego: -1 vida</t>
+          <t>—</t>
         </is>
       </c>
       <c r="F30" t="b">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -2042,10 +2018,10 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -2055,29 +2031,29 @@
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>ATAQUE CRITICO (Éxito) | Ataque Crítico: 0 absorbido, 3 a vida (vida ahora 2)</t>
+          <t>BUFFO DEFENSA (Éxito) | Bufo Defensa: +1 defensa</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>ATAQUE CRITICO</t>
+          <t>BUFFO DEFENSA</t>
         </is>
       </c>
       <c r="L31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
@@ -2097,10 +2073,10 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -2114,20 +2090,20 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Fuego: -1 vida</t>
+          <t>F; u; e; g; o; :;  ; -; 1;  ; v; i; d; a</t>
         </is>
       </c>
       <c r="F32" t="b">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
@@ -2140,10 +2116,10 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -2153,29 +2129,29 @@
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Ataque critico + robar carta (Éxito) | Ataque Crítico: 0 absorbido, 3 a vida (vida ahora -1) &amp; Robo Carta: ambos roban 1 carta</t>
+          <t>BUFFO SUERTE (Éxito) | Bufo Suerte: activado (4 turnos, limite=4)</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Ataque critico + robar carta</t>
+          <t>BUFFO SUERTE</t>
         </is>
       </c>
       <c r="L33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M33" t="inlineStr">
         <is>
@@ -2195,52 +2171,1253 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>7</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>8</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2</v>
+      </c>
+      <c r="B35" t="n">
+        <v>16</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>BUFFO VIDA PEQUEÑO (Éxito) | Bufo Vida Pequeño: +1 vida (vida ahora 8)</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="n">
+        <v>8</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>8</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>BUFFO VIDA PEQUEÑO</t>
+        </is>
+      </c>
+      <c r="L35" t="n">
+        <v>3</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2</v>
+      </c>
+      <c r="B36" t="n">
+        <v>17</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>Jugador 2</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>BUFFO LIMPIEZA AZAR (Éxito, dado=10) | Limpieza: estados negativos eliminados</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H34" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" t="n">
-        <v>1</v>
-      </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>BUFFO LIMPIEZA AZAR</t>
-        </is>
-      </c>
-      <c r="L34" t="n">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>F; u; e; g; o; :;  ; -; 1;  ; v; i; d; a</t>
+        </is>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>8</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>7</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2</v>
+      </c>
+      <c r="B37" t="n">
+        <v>17</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>CONGELAR CERTERO (Éxito) | Congelar Certero: aplicado (salta turno)</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="n">
+        <v>8</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>7</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>CONGELAR CERTERO</t>
+        </is>
+      </c>
+      <c r="L37" t="n">
+        <v>4</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>CERTERO</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2</v>
+      </c>
+      <c r="B38" t="n">
+        <v>18</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>C; o; n; g; e; l; a; d; o; :;  ; p; i; e; r; d; e;  ; t; u; r; n; o</t>
+        </is>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="n">
+        <v>8</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>7</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2</v>
+      </c>
+      <c r="B39" t="n">
+        <v>19</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>8</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>7</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2</v>
+      </c>
+      <c r="B40" t="n">
+        <v>19</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>SANGRADO AZAR (Éxito, dado=9) | Sangrado Azar: aplicado (dado=10, 1×3 turnos)</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="n">
+        <v>8</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>7</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>SANGRADO AZAR</t>
+        </is>
+      </c>
+      <c r="L40" t="n">
+        <v>2</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>AZAR</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>9</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2</v>
+      </c>
+      <c r="B41" t="n">
+        <v>20</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>S; a; n; g; r; a; d; o; :;  ; -; 1;  ; v; i; d; a</t>
+        </is>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>7</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>7</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2</v>
+      </c>
+      <c r="B42" t="n">
+        <v>20</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>ATAQUE NORMAL + CONGELAR AZAR (Éxito, dado=6) | Ataque Normal: 0 absorbido, 2 a vida (vida ahora 5) &amp; Congelar Azar: aplicado (dado=8, salta turno)</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="n">
+        <v>7</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>5</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>ATAQUE NORMAL + CONGELAR AZAR</t>
+        </is>
+      </c>
+      <c r="L42" t="n">
+        <v>4</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>AZAR</t>
+        </is>
+      </c>
+      <c r="N42" t="n">
+        <v>6</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2</v>
+      </c>
+      <c r="B43" t="n">
+        <v>21</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>C; o; n; g; e; l; a; d; o; :;  ; p; i; e; r; d; e;  ; t; u; r; n; o</t>
+        </is>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" t="n">
+        <v>7</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>5</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2</v>
+      </c>
+      <c r="B44" t="n">
+        <v>22</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>S; a; n; g; r; a; d; o; :;  ; -; 1;  ; v; i; d; a</t>
+        </is>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>6</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>5</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2</v>
+      </c>
+      <c r="B45" t="n">
+        <v>22</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>ATAQUE CRITICO (Éxito) | Ataque Crítico: 0 absorbido, 3 a vida (vida ahora 2)</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="n">
+        <v>6</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>2</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>ATAQUE CRITICO</t>
+        </is>
+      </c>
+      <c r="L45" t="n">
         <v>3</v>
       </c>
-      <c r="M34" t="inlineStr">
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2</v>
+      </c>
+      <c r="B46" t="n">
+        <v>23</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>6</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>2</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2</v>
+      </c>
+      <c r="B47" t="n">
+        <v>23</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>BUFFO VIDA MEDIANO (Éxito) | Bufo Vida Mediano: +2 vida (vida ahora 4)</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="n">
+        <v>6</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>4</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>BUFFO VIDA MEDIANO</t>
+        </is>
+      </c>
+      <c r="L47" t="n">
+        <v>4</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>2</v>
+      </c>
+      <c r="B48" t="n">
+        <v>23</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>BUFFO DEFENSA NORMAL (Éxito) | Bufo Defensa Normal: +2 defensa</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="n">
+        <v>6</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>4</v>
+      </c>
+      <c r="J48" t="n">
+        <v>2</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>BUFFO DEFENSA NORMAL</t>
+        </is>
+      </c>
+      <c r="L48" t="n">
+        <v>2</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>2</v>
+      </c>
+      <c r="B49" t="n">
+        <v>24</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>S; a; n; g; r; a; d; o; :;  ; -; 1;  ; v; i; d; a</t>
+        </is>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>5</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>4</v>
+      </c>
+      <c r="J49" t="n">
+        <v>2</v>
+      </c>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>2</v>
+      </c>
+      <c r="B50" t="n">
+        <v>24</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>ATAQUE NORMAL + SANGRADO CERTERO (Éxito) | Ataque Normal: 2 absorbido por defensa (defensa ahora 0) &amp; Sangrado Certero: aplicado (1×3 turnos)</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="n">
+        <v>5</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>3</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>ATAQUE NORMAL + SANGRADO CERTERO</t>
+        </is>
+      </c>
+      <c r="L50" t="n">
+        <v>5</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>CERTERO</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>2</v>
+      </c>
+      <c r="B51" t="n">
+        <v>25</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>S; a; n; g; r; a; d; o; :;  ; -; 1;  ; v; i; d; a</t>
+        </is>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>5</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>2</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>2</v>
+      </c>
+      <c r="B52" t="n">
+        <v>25</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>ATAQUE LIGERO (Éxito) | Ataque Ligero: 0 absorbido, 1 a vida (vida ahora 4)</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="n">
+        <v>4</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>2</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>ATAQUE LIGERO</t>
+        </is>
+      </c>
+      <c r="L52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>2</v>
+      </c>
+      <c r="B53" t="n">
+        <v>26</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>4</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="n">
+        <v>2</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>2</v>
+      </c>
+      <c r="B54" t="n">
+        <v>27</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>S; a; n; g; r; a; d; o; :;  ; -; 1;  ; v; i; d; a</t>
+        </is>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>4</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>1</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2</v>
+      </c>
+      <c r="B55" t="n">
+        <v>27</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>BUFFO DEFENSA (Éxito) | Bufo Defensa: +1 defensa</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="n">
+        <v>4</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>1</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>BUFFO DEFENSA</t>
+        </is>
+      </c>
+      <c r="L55" t="n">
+        <v>1</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2</v>
+      </c>
+      <c r="B56" t="n">
+        <v>28</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>4</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>2</v>
+      </c>
+      <c r="B57" t="n">
+        <v>28</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>ESQUIVAR AZAR (Éxito, dado=7) | Esquivar Azar: fallido (dado=1)</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="n">
+        <v>4</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>ESQUIVAR AZAR</t>
+        </is>
+      </c>
+      <c r="L57" t="n">
+        <v>1</v>
+      </c>
+      <c r="M57" t="inlineStr">
         <is>
           <t>AZAR</t>
         </is>
       </c>
-      <c r="N34" t="n">
-        <v>10</v>
-      </c>
-      <c r="O34" t="inlineStr">
+      <c r="N57" t="n">
+        <v>7</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Éxito</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>2</v>
+      </c>
+      <c r="B58" t="n">
+        <v>29</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>InicioTurno</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>S; a; n; g; r; a; d; o; :;  ; -; 1;  ; v; i; d; a</t>
+        </is>
+      </c>
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>4</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>2</v>
+      </c>
+      <c r="B59" t="n">
+        <v>29</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Fuego azar +buffo defensa (Éxito, dado=6) | Fuego Azar: fallido (dado=3) &amp; Bufo Defensa: +1 defensa</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>4</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>2</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Fuego azar +buffo defensa</t>
+        </is>
+      </c>
+      <c r="L59" t="n">
+        <v>2</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>AZAR</t>
+        </is>
+      </c>
+      <c r="N59" t="n">
+        <v>6</v>
+      </c>
+      <c r="O59" t="inlineStr">
         <is>
           <t>Éxito</t>
         </is>

</xml_diff>